<commit_message>
Updated the pinout in excel file to include UART0 (ttyPS1)
</commit_message>
<xml_diff>
--- a/ADRV9361z7035 BOB Pins.xlsx
+++ b/ADRV9361z7035 BOB Pins.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+  <si>
+    <t xml:space="preserve">RX</t>
+  </si>
   <si>
     <t xml:space="preserve">GI 0</t>
   </si>
@@ -35,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">3.3 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX</t>
   </si>
   <si>
     <t xml:space="preserve">GO 0</t>
@@ -505,9 +511,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -998,7 +1008,7 @@
   <dimension ref="B2:AJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
+      <selection pane="topLeft" activeCell="X29" activeCellId="0" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1010,597 +1020,602 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="R3" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="0" t="n">
         <v>964</v>
       </c>
-      <c r="AI3" s="1"/>
+      <c r="AI3" s="2"/>
       <c r="AJ3" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <f aca="false">B4 - 2</f>
         <v>57</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <f aca="false">C4 - 2</f>
         <v>55</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <f aca="false">D4 - 2</f>
         <v>53</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <f aca="false">E4 - 2</f>
         <v>51</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <f aca="false">F4 - 2</f>
         <v>49</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <f aca="false">G4 - 2</f>
         <v>47</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <f aca="false">H4 - 2</f>
         <v>45</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="4" t="n">
         <f aca="false">I4 - 2</f>
         <v>43</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="4" t="n">
         <f aca="false">J4 - 2</f>
         <v>41</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="4" t="n">
         <f aca="false">K4 - 2</f>
         <v>39</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="4" t="n">
         <f aca="false">L4 - 2</f>
         <v>37</v>
       </c>
-      <c r="N4" s="5" t="n">
+      <c r="N4" s="6" t="n">
         <f aca="false">M4 - 2</f>
         <v>35</v>
       </c>
-      <c r="O4" s="6" t="n">
+      <c r="O4" s="7" t="n">
         <f aca="false">N4 - 2</f>
         <v>33</v>
       </c>
-      <c r="P4" s="6" t="n">
+      <c r="P4" s="7" t="n">
         <f aca="false">O4 - 2</f>
         <v>31</v>
       </c>
-      <c r="Q4" s="7" t="n">
+      <c r="Q4" s="8" t="n">
         <f aca="false">P4 - 2</f>
         <v>29</v>
       </c>
-      <c r="R4" s="7" t="n">
+      <c r="R4" s="8" t="n">
         <f aca="false">Q4 - 2</f>
         <v>27</v>
       </c>
-      <c r="S4" s="3" t="n">
+      <c r="S4" s="4" t="n">
         <f aca="false">R4 - 2</f>
         <v>25</v>
       </c>
-      <c r="T4" s="3" t="n">
+      <c r="T4" s="4" t="n">
         <f aca="false">S4 - 2</f>
         <v>23</v>
       </c>
-      <c r="U4" s="3" t="n">
+      <c r="U4" s="4" t="n">
         <f aca="false">T4 - 2</f>
         <v>21</v>
       </c>
-      <c r="V4" s="3" t="n">
+      <c r="V4" s="4" t="n">
         <f aca="false">U4 - 2</f>
         <v>19</v>
       </c>
-      <c r="W4" s="8" t="n">
+      <c r="W4" s="9" t="n">
         <f aca="false">V4 - 2</f>
         <v>17</v>
       </c>
-      <c r="X4" s="3" t="n">
+      <c r="X4" s="4" t="n">
         <f aca="false">W4 - 2</f>
         <v>15</v>
       </c>
-      <c r="Y4" s="3" t="n">
+      <c r="Y4" s="4" t="n">
         <f aca="false">X4 - 2</f>
         <v>13</v>
       </c>
-      <c r="Z4" s="3" t="n">
+      <c r="Z4" s="4" t="n">
         <f aca="false">Y4 - 2</f>
         <v>11</v>
       </c>
-      <c r="AA4" s="3" t="n">
+      <c r="AA4" s="4" t="n">
         <f aca="false">Z4 - 2</f>
         <v>9</v>
       </c>
-      <c r="AB4" s="3" t="n">
+      <c r="AB4" s="4" t="n">
         <f aca="false">AA4 - 2</f>
         <v>7</v>
       </c>
-      <c r="AC4" s="3" t="n">
+      <c r="AC4" s="4" t="n">
         <f aca="false">AB4 - 2</f>
         <v>5</v>
       </c>
-      <c r="AD4" s="9" t="n">
+      <c r="AD4" s="10" t="n">
         <f aca="false">AC4 - 2</f>
         <v>3</v>
       </c>
-      <c r="AE4" s="10" t="n">
+      <c r="AE4" s="11" t="n">
         <f aca="false">AD4 - 2</f>
         <v>1</v>
       </c>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI4" s="13"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="14"/>
       <c r="AJ4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14" t="n">
+      <c r="B5" s="15" t="n">
         <v>60</v>
       </c>
-      <c r="C5" s="15" t="n">
+      <c r="C5" s="16" t="n">
         <f aca="false">B5 - 2</f>
         <v>58</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="16" t="n">
         <f aca="false">C5 - 2</f>
         <v>56</v>
       </c>
-      <c r="E5" s="15" t="n">
+      <c r="E5" s="16" t="n">
         <f aca="false">D5 - 2</f>
         <v>54</v>
       </c>
-      <c r="F5" s="15" t="n">
+      <c r="F5" s="16" t="n">
         <f aca="false">E5 - 2</f>
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="n">
+      <c r="G5" s="17" t="n">
         <f aca="false">F5 - 2</f>
         <v>50</v>
       </c>
-      <c r="H5" s="15" t="n">
+      <c r="H5" s="16" t="n">
         <f aca="false">G5 - 2</f>
         <v>48</v>
       </c>
-      <c r="I5" s="15" t="n">
+      <c r="I5" s="16" t="n">
         <f aca="false">H5 - 2</f>
         <v>46</v>
       </c>
-      <c r="J5" s="15" t="n">
+      <c r="J5" s="16" t="n">
         <f aca="false">I5 - 2</f>
         <v>44</v>
       </c>
-      <c r="K5" s="15" t="n">
+      <c r="K5" s="16" t="n">
         <f aca="false">J5 - 2</f>
         <v>42</v>
       </c>
-      <c r="L5" s="15" t="n">
+      <c r="L5" s="16" t="n">
         <f aca="false">K5 - 2</f>
         <v>40</v>
       </c>
-      <c r="M5" s="15" t="n">
+      <c r="M5" s="16" t="n">
         <f aca="false">L5 - 2</f>
         <v>38</v>
       </c>
-      <c r="N5" s="17" t="n">
+      <c r="N5" s="18" t="n">
         <f aca="false">M5 - 2</f>
         <v>36</v>
       </c>
-      <c r="O5" s="18" t="n">
+      <c r="O5" s="19" t="n">
         <f aca="false">N5 - 2</f>
         <v>34</v>
       </c>
-      <c r="P5" s="18" t="n">
+      <c r="P5" s="19" t="n">
         <f aca="false">O5 - 2</f>
         <v>32</v>
       </c>
-      <c r="Q5" s="19" t="n">
+      <c r="Q5" s="20" t="n">
         <f aca="false">P5 - 2</f>
         <v>30</v>
       </c>
-      <c r="R5" s="19" t="n">
+      <c r="R5" s="20" t="n">
         <f aca="false">Q5 - 2</f>
         <v>28</v>
       </c>
-      <c r="S5" s="15" t="n">
+      <c r="S5" s="16" t="n">
         <f aca="false">R5 - 2</f>
         <v>26</v>
       </c>
-      <c r="T5" s="15" t="n">
+      <c r="T5" s="16" t="n">
         <f aca="false">S5 - 2</f>
         <v>24</v>
       </c>
-      <c r="U5" s="15" t="n">
+      <c r="U5" s="16" t="n">
         <f aca="false">T5 - 2</f>
         <v>22</v>
       </c>
-      <c r="V5" s="15" t="n">
+      <c r="V5" s="16" t="n">
         <f aca="false">U5 - 2</f>
         <v>20</v>
       </c>
-      <c r="W5" s="20" t="n">
+      <c r="W5" s="21" t="n">
         <f aca="false">V5 - 2</f>
         <v>18</v>
       </c>
-      <c r="X5" s="21" t="n">
+      <c r="X5" s="22" t="n">
         <f aca="false">W5 - 2</f>
         <v>16</v>
       </c>
-      <c r="Y5" s="22" t="n">
+      <c r="Y5" s="23" t="n">
         <f aca="false">X5 - 2</f>
         <v>14</v>
       </c>
-      <c r="Z5" s="15" t="n">
+      <c r="Z5" s="16" t="n">
         <f aca="false">Y5 - 2</f>
         <v>12</v>
       </c>
-      <c r="AA5" s="15" t="n">
+      <c r="AA5" s="16" t="n">
         <f aca="false">Z5 - 2</f>
         <v>10</v>
       </c>
-      <c r="AB5" s="15" t="n">
+      <c r="AB5" s="16" t="n">
         <f aca="false">AA5 - 2</f>
         <v>8</v>
       </c>
-      <c r="AC5" s="15" t="n">
+      <c r="AC5" s="16" t="n">
         <f aca="false">AB5 - 2</f>
         <v>6</v>
       </c>
-      <c r="AD5" s="23" t="n">
+      <c r="AD5" s="24" t="n">
         <f aca="false">AC5 - 2</f>
         <v>4</v>
       </c>
-      <c r="AE5" s="24" t="n">
+      <c r="AE5" s="25" t="n">
         <f aca="false">AD5 - 2</f>
         <v>2</v>
       </c>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AI5" s="25"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AI5" s="26"/>
       <c r="AJ5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="n">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="n">
         <v>966</v>
       </c>
-      <c r="F6" s="11" t="n">
+      <c r="F6" s="12" t="n">
         <v>965</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="R6" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AI6" s="26"/>
+        <v>9</v>
+      </c>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AI6" s="27"/>
       <c r="AJ6" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11" t="n">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12" t="n">
         <v>967</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="11" t="n">
+      <c r="K7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="12" t="n">
         <v>972</v>
       </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11" t="n">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12" t="n">
         <v>973</v>
       </c>
-      <c r="P7" s="11" t="n">
+      <c r="P7" s="12" t="n">
         <v>975</v>
       </c>
-      <c r="Q7" s="11" t="n">
+      <c r="Q7" s="12" t="n">
         <v>963</v>
       </c>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V7" s="11" t="n">
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" s="12" t="n">
         <v>979</v>
       </c>
-      <c r="W7" s="11" t="n">
+      <c r="W7" s="12" t="n">
         <v>977</v>
       </c>
-      <c r="X7" s="11" t="n">
+      <c r="X7" s="12" t="n">
         <v>989</v>
       </c>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="11"/>
-      <c r="AG7" s="11"/>
-      <c r="AI7" s="27"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="12"/>
+      <c r="AI7" s="28"/>
       <c r="AJ7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="28" t="n">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="29" t="n">
         <v>32</v>
       </c>
-      <c r="J8" s="29" t="n">
+      <c r="J8" s="30" t="n">
         <f aca="false">I8 -2</f>
         <v>30</v>
       </c>
-      <c r="K8" s="29" t="n">
+      <c r="K8" s="30" t="n">
         <f aca="false">J8 -2</f>
         <v>28</v>
       </c>
-      <c r="L8" s="29" t="n">
+      <c r="L8" s="30" t="n">
         <f aca="false">K8 -2</f>
         <v>26</v>
       </c>
-      <c r="M8" s="30" t="n">
+      <c r="M8" s="31" t="n">
         <f aca="false">L8 -2</f>
         <v>24</v>
       </c>
-      <c r="N8" s="30" t="n">
+      <c r="N8" s="31" t="n">
         <f aca="false">M8 -2</f>
         <v>22</v>
       </c>
-      <c r="O8" s="29" t="n">
+      <c r="O8" s="30" t="n">
         <f aca="false">N8 -2</f>
         <v>20</v>
       </c>
-      <c r="P8" s="29" t="n">
+      <c r="P8" s="30" t="n">
         <f aca="false">O8 -2</f>
         <v>18</v>
       </c>
-      <c r="Q8" s="31" t="n">
+      <c r="Q8" s="32" t="n">
         <f aca="false">P8 -2</f>
         <v>16</v>
       </c>
-      <c r="R8" s="32" t="n">
+      <c r="R8" s="33" t="n">
         <f aca="false">Q8 -2</f>
         <v>14</v>
       </c>
-      <c r="S8" s="33" t="n">
+      <c r="S8" s="34" t="n">
         <f aca="false">R8 -2</f>
         <v>12</v>
       </c>
-      <c r="T8" s="33" t="n">
+      <c r="T8" s="34" t="n">
         <f aca="false">S8 -2</f>
         <v>10</v>
       </c>
-      <c r="U8" s="29" t="n">
+      <c r="U8" s="30" t="n">
         <f aca="false">T8 -2</f>
         <v>8</v>
       </c>
-      <c r="V8" s="29" t="n">
+      <c r="V8" s="30" t="n">
         <f aca="false">U8 -2</f>
         <v>6</v>
       </c>
-      <c r="W8" s="34" t="n">
+      <c r="W8" s="35" t="n">
         <f aca="false">V8 -2</f>
         <v>4</v>
       </c>
-      <c r="X8" s="35" t="n">
+      <c r="X8" s="36" t="n">
         <f aca="false">W8 -2</f>
         <v>2</v>
       </c>
-      <c r="Z8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-      <c r="AI8" s="36"/>
+      <c r="Z8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="12"/>
+      <c r="AI8" s="37"/>
       <c r="AJ8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="37" t="n">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="38" t="n">
         <v>31</v>
       </c>
-      <c r="J9" s="38" t="n">
+      <c r="J9" s="39" t="n">
         <f aca="false">I9 - 2</f>
         <v>29</v>
       </c>
-      <c r="K9" s="39" t="n">
+      <c r="K9" s="40" t="n">
         <f aca="false">J9 - 2</f>
         <v>27</v>
       </c>
-      <c r="L9" s="39" t="n">
+      <c r="L9" s="40" t="n">
         <f aca="false">K9 - 2</f>
         <v>25</v>
       </c>
-      <c r="M9" s="20" t="n">
+      <c r="M9" s="21" t="n">
         <f aca="false">L9 - 2</f>
         <v>23</v>
       </c>
-      <c r="N9" s="40" t="n">
+      <c r="N9" s="41" t="n">
         <f aca="false">M9 - 2</f>
         <v>21</v>
       </c>
-      <c r="O9" s="39" t="n">
+      <c r="O9" s="40" t="n">
         <f aca="false">N9 - 2</f>
         <v>19</v>
       </c>
-      <c r="P9" s="39" t="n">
+      <c r="P9" s="40" t="n">
         <f aca="false">O9 - 2</f>
         <v>17</v>
       </c>
-      <c r="Q9" s="41" t="n">
+      <c r="Q9" s="42" t="n">
         <f aca="false">P9 - 2</f>
         <v>15</v>
       </c>
-      <c r="R9" s="42" t="n">
+      <c r="R9" s="43" t="n">
         <f aca="false">Q9 - 2</f>
         <v>13</v>
       </c>
-      <c r="S9" s="20" t="n">
+      <c r="S9" s="21" t="n">
         <f aca="false">R9 - 2</f>
         <v>11</v>
       </c>
-      <c r="T9" s="17" t="n">
+      <c r="T9" s="18" t="n">
         <f aca="false">S9 - 2</f>
         <v>9</v>
       </c>
-      <c r="U9" s="39" t="n">
+      <c r="U9" s="40" t="n">
         <f aca="false">T9 - 2</f>
         <v>7</v>
       </c>
-      <c r="V9" s="39" t="n">
+      <c r="V9" s="40" t="n">
         <f aca="false">U9 - 2</f>
         <v>5</v>
       </c>
-      <c r="W9" s="43" t="n">
+      <c r="W9" s="44" t="n">
         <f aca="false">V9 - 2</f>
         <v>3</v>
       </c>
-      <c r="X9" s="44" t="n">
+      <c r="X9" s="45" t="n">
         <f aca="false">W9 - 2</f>
         <v>1</v>
       </c>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11"/>
-      <c r="AI9" s="45"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="12"/>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="12"/>
+      <c r="AI9" s="46"/>
       <c r="AJ9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="11" t="s">
+      <c r="L10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11" t="s">
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="V10" s="11" t="n">
+      <c r="P10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="V10" s="12" t="n">
         <v>971</v>
       </c>
-      <c r="W10" s="11" t="n">
+      <c r="W10" s="12" t="n">
         <v>974</v>
       </c>
-      <c r="X10" s="11" t="n">
+      <c r="X10" s="12" t="n">
         <v>976</v>
       </c>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
-      <c r="AI10" s="46"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AI10" s="47"/>
       <c r="AJ10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="0" t="n">
         <v>987</v>
       </c>
@@ -1623,220 +1638,220 @@
         <v>981</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-      <c r="AI11" s="47"/>
+        <v>27</v>
+      </c>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AI11" s="48"/>
       <c r="AJ11" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="48" t="n">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="49" t="n">
         <v>32</v>
       </c>
-      <c r="J12" s="49" t="n">
+      <c r="J12" s="50" t="n">
         <f aca="false">I12 -2</f>
         <v>30</v>
       </c>
-      <c r="K12" s="50" t="n">
+      <c r="K12" s="51" t="n">
         <f aca="false">J12 -2</f>
         <v>28</v>
       </c>
-      <c r="L12" s="50" t="n">
+      <c r="L12" s="51" t="n">
         <f aca="false">K12 -2</f>
         <v>26</v>
       </c>
-      <c r="M12" s="8" t="n">
+      <c r="M12" s="9" t="n">
         <f aca="false">L12 -2</f>
         <v>24</v>
       </c>
-      <c r="N12" s="51" t="n">
+      <c r="N12" s="52" t="n">
         <f aca="false">M12 -2</f>
         <v>22</v>
       </c>
-      <c r="O12" s="29" t="n">
+      <c r="O12" s="30" t="n">
         <f aca="false">N12 -2</f>
         <v>20</v>
       </c>
-      <c r="P12" s="29" t="n">
+      <c r="P12" s="30" t="n">
         <f aca="false">O12 -2</f>
         <v>18</v>
       </c>
-      <c r="Q12" s="29" t="n">
+      <c r="Q12" s="30" t="n">
         <f aca="false">P12 -2</f>
         <v>16</v>
       </c>
-      <c r="R12" s="29" t="n">
+      <c r="R12" s="30" t="n">
         <f aca="false">Q12 -2</f>
         <v>14</v>
       </c>
-      <c r="S12" s="8" t="n">
+      <c r="S12" s="9" t="n">
         <f aca="false">R12 -2</f>
         <v>12</v>
       </c>
-      <c r="T12" s="5" t="n">
+      <c r="T12" s="6" t="n">
         <f aca="false">S12 -2</f>
         <v>10</v>
       </c>
-      <c r="U12" s="29" t="n">
+      <c r="U12" s="30" t="n">
         <f aca="false">T12 -2</f>
         <v>8</v>
       </c>
-      <c r="V12" s="29" t="n">
+      <c r="V12" s="30" t="n">
         <f aca="false">U12 -2</f>
         <v>6</v>
       </c>
-      <c r="W12" s="29" t="n">
+      <c r="W12" s="30" t="n">
         <f aca="false">V12 -2</f>
         <v>4</v>
       </c>
-      <c r="X12" s="52" t="n">
+      <c r="X12" s="53" t="n">
         <f aca="false">W12 -2</f>
         <v>2</v>
       </c>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AI12" s="53"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AI12" s="54"/>
       <c r="AJ12" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="54" t="n">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="55" t="n">
         <v>31</v>
       </c>
-      <c r="J13" s="55" t="n">
+      <c r="J13" s="56" t="n">
         <f aca="false">I13 - 2</f>
         <v>29</v>
       </c>
-      <c r="K13" s="39" t="n">
+      <c r="K13" s="40" t="n">
         <f aca="false">J13 - 2</f>
         <v>27</v>
       </c>
-      <c r="L13" s="39" t="n">
+      <c r="L13" s="40" t="n">
         <f aca="false">K13 - 2</f>
         <v>25</v>
       </c>
-      <c r="M13" s="56" t="n">
+      <c r="M13" s="57" t="n">
         <f aca="false">L13 - 2</f>
         <v>23</v>
       </c>
-      <c r="N13" s="56" t="n">
+      <c r="N13" s="57" t="n">
         <f aca="false">M13 - 2</f>
         <v>21</v>
       </c>
-      <c r="O13" s="57" t="n">
+      <c r="O13" s="58" t="n">
         <f aca="false">N13 - 2</f>
         <v>19</v>
       </c>
-      <c r="P13" s="39" t="n">
+      <c r="P13" s="40" t="n">
         <f aca="false">O13 - 2</f>
         <v>17</v>
       </c>
-      <c r="Q13" s="39" t="n">
+      <c r="Q13" s="40" t="n">
         <f aca="false">P13 - 2</f>
         <v>15</v>
       </c>
-      <c r="R13" s="39" t="n">
+      <c r="R13" s="40" t="n">
         <f aca="false">Q13 - 2</f>
         <v>13</v>
       </c>
-      <c r="S13" s="58" t="n">
+      <c r="S13" s="59" t="n">
         <f aca="false">R13 - 2</f>
         <v>11</v>
       </c>
-      <c r="T13" s="39" t="n">
+      <c r="T13" s="40" t="n">
         <f aca="false">S13 - 2</f>
         <v>9</v>
       </c>
-      <c r="U13" s="39" t="n">
+      <c r="U13" s="40" t="n">
         <f aca="false">T13 - 2</f>
         <v>7</v>
       </c>
-      <c r="V13" s="39" t="n">
+      <c r="V13" s="40" t="n">
         <f aca="false">U13 - 2</f>
         <v>5</v>
       </c>
-      <c r="W13" s="39" t="n">
+      <c r="W13" s="40" t="n">
         <f aca="false">V13 - 2</f>
         <v>3</v>
       </c>
-      <c r="X13" s="59" t="n">
+      <c r="X13" s="60" t="n">
         <f aca="false">W13 - 2</f>
         <v>1</v>
       </c>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-      <c r="AI13" s="60"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="12"/>
+      <c r="AI13" s="61"/>
       <c r="AJ13" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>980</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>968</v>
@@ -1872,357 +1887,357 @@
         <v>982</v>
       </c>
       <c r="X14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12"/>
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="12"/>
+      <c r="AI14" s="62"/>
+      <c r="AJ14" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="12"/>
+      <c r="AF15" s="12"/>
+      <c r="AG15" s="12"/>
+      <c r="AI15" s="63"/>
+      <c r="AJ15" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="64" t="n">
         <v>32</v>
       </c>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AI14" s="61"/>
-      <c r="AJ14" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-      <c r="AI15" s="62"/>
-      <c r="AJ15" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="63" t="n">
-        <v>32</v>
-      </c>
-      <c r="J16" s="64" t="n">
+      <c r="J16" s="65" t="n">
         <f aca="false">I16 -2</f>
         <v>30</v>
       </c>
-      <c r="K16" s="65" t="n">
+      <c r="K16" s="66" t="n">
         <f aca="false">J16 -2</f>
         <v>28</v>
       </c>
-      <c r="L16" s="65" t="n">
+      <c r="L16" s="66" t="n">
         <f aca="false">K16 -2</f>
         <v>26</v>
       </c>
-      <c r="M16" s="66" t="n">
+      <c r="M16" s="67" t="n">
         <f aca="false">L16 -2</f>
         <v>24</v>
       </c>
-      <c r="N16" s="66" t="n">
+      <c r="N16" s="67" t="n">
         <f aca="false">M16 -2</f>
         <v>22</v>
       </c>
-      <c r="O16" s="65" t="n">
+      <c r="O16" s="66" t="n">
         <f aca="false">N16 -2</f>
         <v>20</v>
       </c>
-      <c r="P16" s="65" t="n">
+      <c r="P16" s="66" t="n">
         <f aca="false">O16 -2</f>
         <v>18</v>
       </c>
-      <c r="Q16" s="65" t="n">
+      <c r="Q16" s="66" t="n">
         <f aca="false">P16 -2</f>
         <v>16</v>
       </c>
-      <c r="R16" s="65" t="n">
+      <c r="R16" s="66" t="n">
         <f aca="false">Q16 -2</f>
         <v>14</v>
       </c>
-      <c r="S16" s="67" t="n">
+      <c r="S16" s="68" t="n">
         <f aca="false">R16 -2</f>
         <v>12</v>
       </c>
-      <c r="T16" s="67" t="n">
+      <c r="T16" s="68" t="n">
         <f aca="false">S16 -2</f>
         <v>10</v>
       </c>
-      <c r="U16" s="65" t="n">
+      <c r="U16" s="66" t="n">
         <f aca="false">T16 -2</f>
         <v>8</v>
       </c>
-      <c r="V16" s="65" t="n">
+      <c r="V16" s="66" t="n">
         <f aca="false">U16 -2</f>
         <v>6</v>
       </c>
-      <c r="W16" s="65" t="n">
+      <c r="W16" s="66" t="n">
         <f aca="false">V16 -2</f>
         <v>4</v>
       </c>
-      <c r="X16" s="68" t="n">
+      <c r="X16" s="69" t="n">
         <f aca="false">W16 -2</f>
         <v>2</v>
       </c>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AI16" s="69"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="12"/>
+      <c r="AI16" s="70"/>
       <c r="AJ16" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I17" s="70" t="n">
+      <c r="I17" s="71" t="n">
         <v>31</v>
       </c>
-      <c r="J17" s="71" t="n">
+      <c r="J17" s="72" t="n">
         <f aca="false">I17 - 2</f>
         <v>29</v>
       </c>
-      <c r="K17" s="72" t="n">
+      <c r="K17" s="73" t="n">
         <f aca="false">J17 - 2</f>
         <v>27</v>
       </c>
-      <c r="L17" s="72" t="n">
+      <c r="L17" s="73" t="n">
         <f aca="false">K17 - 2</f>
         <v>25</v>
       </c>
-      <c r="M17" s="20" t="n">
+      <c r="M17" s="21" t="n">
         <f aca="false">L17 - 2</f>
         <v>23</v>
       </c>
-      <c r="N17" s="40" t="n">
+      <c r="N17" s="41" t="n">
         <f aca="false">M17 - 2</f>
         <v>21</v>
       </c>
-      <c r="O17" s="72" t="n">
+      <c r="O17" s="73" t="n">
         <f aca="false">N17 - 2</f>
         <v>19</v>
       </c>
-      <c r="P17" s="72" t="n">
+      <c r="P17" s="73" t="n">
         <f aca="false">O17 - 2</f>
         <v>17</v>
       </c>
-      <c r="Q17" s="72" t="n">
+      <c r="Q17" s="73" t="n">
         <f aca="false">P17 - 2</f>
         <v>15</v>
       </c>
-      <c r="R17" s="72" t="n">
+      <c r="R17" s="73" t="n">
         <f aca="false">Q17 - 2</f>
         <v>13</v>
       </c>
-      <c r="S17" s="20" t="n">
+      <c r="S17" s="21" t="n">
         <f aca="false">R17 - 2</f>
         <v>11</v>
       </c>
-      <c r="T17" s="17" t="n">
+      <c r="T17" s="18" t="n">
         <f aca="false">S17 - 2</f>
         <v>9</v>
       </c>
-      <c r="U17" s="72" t="n">
+      <c r="U17" s="73" t="n">
         <f aca="false">T17 - 2</f>
         <v>7</v>
       </c>
-      <c r="V17" s="72" t="n">
+      <c r="V17" s="73" t="n">
         <f aca="false">U17 - 2</f>
         <v>5</v>
       </c>
-      <c r="W17" s="72" t="n">
+      <c r="W17" s="73" t="n">
         <f aca="false">V17 - 2</f>
         <v>3</v>
       </c>
-      <c r="X17" s="73" t="n">
+      <c r="X17" s="74" t="n">
         <f aca="false">W17 - 2</f>
         <v>1</v>
       </c>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AI17" s="74"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AI17" s="75"/>
       <c r="AJ17" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI18" s="75"/>
+      <c r="AI18" s="76"/>
       <c r="AJ18" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI19" s="76"/>
+      <c r="AI19" s="77"/>
       <c r="AJ19" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="77" t="n">
+      <c r="I20" s="78" t="n">
         <v>32</v>
       </c>
-      <c r="J20" s="65" t="n">
+      <c r="J20" s="66" t="n">
         <f aca="false">I20 -2</f>
         <v>30</v>
       </c>
-      <c r="K20" s="65" t="n">
+      <c r="K20" s="66" t="n">
         <f aca="false">J20 -2</f>
         <v>28</v>
       </c>
-      <c r="L20" s="65" t="n">
+      <c r="L20" s="66" t="n">
         <f aca="false">K20 -2</f>
         <v>26</v>
       </c>
-      <c r="M20" s="8" t="n">
+      <c r="M20" s="9" t="n">
         <f aca="false">L20 -2</f>
         <v>24</v>
       </c>
-      <c r="N20" s="51" t="n">
+      <c r="N20" s="52" t="n">
         <f aca="false">M20 -2</f>
         <v>22</v>
       </c>
-      <c r="O20" s="65" t="n">
+      <c r="O20" s="66" t="n">
         <f aca="false">N20 -2</f>
         <v>20</v>
       </c>
-      <c r="P20" s="65" t="n">
+      <c r="P20" s="66" t="n">
         <f aca="false">O20 -2</f>
         <v>18</v>
       </c>
-      <c r="Q20" s="65" t="n">
+      <c r="Q20" s="66" t="n">
         <f aca="false">P20 -2</f>
         <v>16</v>
       </c>
-      <c r="R20" s="65" t="n">
+      <c r="R20" s="66" t="n">
         <f aca="false">Q20 -2</f>
         <v>14</v>
       </c>
-      <c r="S20" s="8" t="n">
+      <c r="S20" s="9" t="n">
         <f aca="false">R20 -2</f>
         <v>12</v>
       </c>
-      <c r="T20" s="5" t="n">
+      <c r="T20" s="6" t="n">
         <f aca="false">S20 -2</f>
         <v>10</v>
       </c>
-      <c r="U20" s="65" t="n">
+      <c r="U20" s="66" t="n">
         <f aca="false">T20 -2</f>
         <v>8</v>
       </c>
-      <c r="V20" s="65" t="n">
+      <c r="V20" s="66" t="n">
         <f aca="false">U20 -2</f>
         <v>6</v>
       </c>
-      <c r="W20" s="65" t="n">
+      <c r="W20" s="66" t="n">
         <f aca="false">V20 -2</f>
         <v>4</v>
       </c>
-      <c r="X20" s="68" t="n">
+      <c r="X20" s="69" t="n">
         <f aca="false">W20 -2</f>
         <v>2</v>
       </c>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI20" s="78"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI20" s="79"/>
       <c r="AJ20" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="79" t="n">
+      <c r="I21" s="80" t="n">
         <v>31</v>
       </c>
-      <c r="J21" s="71" t="n">
+      <c r="J21" s="72" t="n">
         <f aca="false">I21 - 2</f>
         <v>29</v>
       </c>
-      <c r="K21" s="80" t="n">
+      <c r="K21" s="81" t="n">
         <f aca="false">J21 - 2</f>
         <v>27</v>
       </c>
-      <c r="L21" s="80" t="n">
+      <c r="L21" s="81" t="n">
         <f aca="false">K21 - 2</f>
         <v>25</v>
       </c>
-      <c r="M21" s="38" t="n">
+      <c r="M21" s="39" t="n">
         <f aca="false">L21 - 2</f>
         <v>23</v>
       </c>
-      <c r="N21" s="56" t="n">
+      <c r="N21" s="57" t="n">
         <f aca="false">M21 - 2</f>
         <v>21</v>
       </c>
-      <c r="O21" s="72" t="n">
+      <c r="O21" s="73" t="n">
         <f aca="false">N21 - 2</f>
         <v>19</v>
       </c>
-      <c r="P21" s="72" t="n">
+      <c r="P21" s="73" t="n">
         <f aca="false">O21 - 2</f>
         <v>17</v>
       </c>
-      <c r="Q21" s="72" t="n">
+      <c r="Q21" s="73" t="n">
         <f aca="false">P21 - 2</f>
         <v>15</v>
       </c>
-      <c r="R21" s="72" t="n">
+      <c r="R21" s="73" t="n">
         <f aca="false">Q21 - 2</f>
         <v>13</v>
       </c>
-      <c r="S21" s="56" t="n">
+      <c r="S21" s="57" t="n">
         <f aca="false">R21 - 2</f>
         <v>11</v>
       </c>
-      <c r="T21" s="56" t="n">
+      <c r="T21" s="57" t="n">
         <f aca="false">S21 - 2</f>
         <v>9</v>
       </c>
-      <c r="U21" s="72" t="n">
+      <c r="U21" s="73" t="n">
         <f aca="false">T21 - 2</f>
         <v>7</v>
       </c>
-      <c r="V21" s="72" t="n">
+      <c r="V21" s="73" t="n">
         <f aca="false">U21 - 2</f>
         <v>5</v>
       </c>
-      <c r="W21" s="72" t="n">
+      <c r="W21" s="73" t="n">
         <f aca="false">V21 - 2</f>
         <v>3</v>
       </c>
-      <c r="X21" s="73" t="n">
+      <c r="X21" s="74" t="n">
         <f aca="false">W21 - 2</f>
         <v>1</v>
       </c>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AI21" s="81"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+      <c r="AI21" s="82"/>
       <c r="AJ21" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M22" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>906</v>
@@ -2233,319 +2248,319 @@
       <c r="T22" s="0" t="n">
         <v>919</v>
       </c>
-      <c r="AI22" s="82"/>
+      <c r="AI22" s="83"/>
       <c r="AJ22" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI23" s="83"/>
+      <c r="AI23" s="84"/>
       <c r="AJ23" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="C24" s="84" t="n">
+      <c r="C24" s="85" t="n">
         <f aca="false">B24 - 2</f>
         <v>57</v>
       </c>
-      <c r="D24" s="84" t="n">
+      <c r="D24" s="85" t="n">
         <f aca="false">C24 - 2</f>
         <v>55</v>
       </c>
-      <c r="E24" s="4" t="n">
+      <c r="E24" s="5" t="n">
         <f aca="false">D24 - 2</f>
         <v>53</v>
       </c>
-      <c r="F24" s="85" t="n">
+      <c r="F24" s="86" t="n">
         <f aca="false">E24 - 2</f>
         <v>51</v>
       </c>
-      <c r="G24" s="85" t="n">
+      <c r="G24" s="86" t="n">
         <f aca="false">F24 - 2</f>
         <v>49</v>
       </c>
-      <c r="H24" s="85" t="n">
+      <c r="H24" s="86" t="n">
         <f aca="false">G24 - 2</f>
         <v>47</v>
       </c>
-      <c r="I24" s="85" t="n">
+      <c r="I24" s="86" t="n">
         <f aca="false">H24 - 2</f>
         <v>45</v>
       </c>
-      <c r="J24" s="85" t="n">
+      <c r="J24" s="86" t="n">
         <f aca="false">I24 - 2</f>
         <v>43</v>
       </c>
-      <c r="K24" s="85" t="n">
+      <c r="K24" s="86" t="n">
         <f aca="false">J24 - 2</f>
         <v>41</v>
       </c>
-      <c r="L24" s="5" t="n">
+      <c r="L24" s="6" t="n">
         <f aca="false">K24 - 2</f>
         <v>39</v>
       </c>
-      <c r="M24" s="86" t="n">
+      <c r="M24" s="87" t="n">
         <f aca="false">L24 - 2</f>
         <v>37</v>
       </c>
-      <c r="N24" s="86" t="n">
+      <c r="N24" s="87" t="n">
         <f aca="false">M24 - 2</f>
         <v>35</v>
       </c>
-      <c r="O24" s="86" t="n">
+      <c r="O24" s="87" t="n">
         <f aca="false">N24 - 2</f>
         <v>33</v>
       </c>
-      <c r="P24" s="86" t="n">
+      <c r="P24" s="87" t="n">
         <f aca="false">O24 - 2</f>
         <v>31</v>
       </c>
-      <c r="Q24" s="86" t="n">
+      <c r="Q24" s="87" t="n">
         <f aca="false">P24 - 2</f>
         <v>29</v>
       </c>
-      <c r="R24" s="86" t="n">
+      <c r="R24" s="87" t="n">
         <f aca="false">Q24 - 2</f>
         <v>27</v>
       </c>
-      <c r="S24" s="86" t="n">
+      <c r="S24" s="87" t="n">
         <f aca="false">R24 - 2</f>
         <v>25</v>
       </c>
-      <c r="T24" s="86" t="n">
+      <c r="T24" s="87" t="n">
         <f aca="false">S24 - 2</f>
         <v>23</v>
       </c>
-      <c r="U24" s="86" t="n">
+      <c r="U24" s="87" t="n">
         <f aca="false">T24 - 2</f>
         <v>21</v>
       </c>
-      <c r="V24" s="86" t="n">
+      <c r="V24" s="87" t="n">
         <f aca="false">U24 - 2</f>
         <v>19</v>
       </c>
-      <c r="W24" s="8" t="n">
+      <c r="W24" s="9" t="n">
         <f aca="false">V24 - 2</f>
         <v>17</v>
       </c>
-      <c r="X24" s="87" t="n">
+      <c r="X24" s="88" t="n">
         <f aca="false">W24 - 2</f>
         <v>15</v>
       </c>
-      <c r="Y24" s="87" t="n">
+      <c r="Y24" s="88" t="n">
         <f aca="false">X24 - 2</f>
         <v>13</v>
       </c>
-      <c r="Z24" s="88" t="n">
+      <c r="Z24" s="89" t="n">
         <f aca="false">Y24 - 2</f>
         <v>11</v>
       </c>
-      <c r="AA24" s="88" t="n">
+      <c r="AA24" s="89" t="n">
         <f aca="false">Z24 - 2</f>
         <v>9</v>
       </c>
-      <c r="AB24" s="86" t="n">
+      <c r="AB24" s="87" t="n">
         <f aca="false">AA24 - 2</f>
         <v>7</v>
       </c>
-      <c r="AC24" s="86" t="n">
+      <c r="AC24" s="87" t="n">
         <f aca="false">AB24 - 2</f>
         <v>5</v>
       </c>
-      <c r="AD24" s="31" t="n">
+      <c r="AD24" s="32" t="n">
         <f aca="false">AC24 - 2</f>
         <v>3</v>
       </c>
-      <c r="AE24" s="10" t="n">
+      <c r="AE24" s="11" t="n">
         <f aca="false">AD24 - 2</f>
         <v>1</v>
       </c>
-      <c r="AF24" s="11"/>
-      <c r="AG24" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI24" s="89"/>
+      <c r="AF24" s="12"/>
+      <c r="AG24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI24" s="90"/>
       <c r="AJ24" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="n">
+      <c r="B25" s="15" t="n">
         <v>60</v>
       </c>
-      <c r="C25" s="90" t="n">
+      <c r="C25" s="91" t="n">
         <f aca="false">B25 - 2</f>
         <v>58</v>
       </c>
-      <c r="D25" s="90" t="n">
+      <c r="D25" s="91" t="n">
         <f aca="false">C25 - 2</f>
         <v>56</v>
       </c>
-      <c r="E25" s="16" t="n">
+      <c r="E25" s="17" t="n">
         <f aca="false">D25 - 2</f>
         <v>54</v>
       </c>
-      <c r="F25" s="91" t="n">
+      <c r="F25" s="92" t="n">
         <f aca="false">E25 - 2</f>
         <v>52</v>
       </c>
-      <c r="G25" s="91" t="n">
+      <c r="G25" s="92" t="n">
         <f aca="false">F25 - 2</f>
         <v>50</v>
       </c>
-      <c r="H25" s="91" t="n">
+      <c r="H25" s="92" t="n">
         <f aca="false">G25 - 2</f>
         <v>48</v>
       </c>
-      <c r="I25" s="91" t="n">
+      <c r="I25" s="92" t="n">
         <f aca="false">H25 - 2</f>
         <v>46</v>
       </c>
-      <c r="J25" s="91" t="n">
+      <c r="J25" s="92" t="n">
         <f aca="false">I25 - 2</f>
         <v>44</v>
       </c>
-      <c r="K25" s="91" t="n">
+      <c r="K25" s="92" t="n">
         <f aca="false">J25 - 2</f>
         <v>42</v>
       </c>
-      <c r="L25" s="17" t="n">
+      <c r="L25" s="18" t="n">
         <f aca="false">K25 - 2</f>
         <v>40</v>
       </c>
-      <c r="M25" s="92" t="n">
+      <c r="M25" s="93" t="n">
         <f aca="false">L25 - 2</f>
         <v>38</v>
       </c>
-      <c r="N25" s="92" t="n">
+      <c r="N25" s="93" t="n">
         <f aca="false">M25 - 2</f>
         <v>36</v>
       </c>
-      <c r="O25" s="92" t="n">
+      <c r="O25" s="93" t="n">
         <f aca="false">N25 - 2</f>
         <v>34</v>
       </c>
-      <c r="P25" s="92" t="n">
+      <c r="P25" s="93" t="n">
         <f aca="false">O25 - 2</f>
         <v>32</v>
       </c>
-      <c r="Q25" s="92" t="n">
+      <c r="Q25" s="93" t="n">
         <f aca="false">P25 - 2</f>
         <v>30</v>
       </c>
-      <c r="R25" s="92" t="n">
+      <c r="R25" s="93" t="n">
         <f aca="false">Q25 - 2</f>
         <v>28</v>
       </c>
-      <c r="S25" s="92" t="n">
+      <c r="S25" s="93" t="n">
         <f aca="false">R25 - 2</f>
         <v>26</v>
       </c>
-      <c r="T25" s="92" t="n">
+      <c r="T25" s="93" t="n">
         <f aca="false">S25 - 2</f>
         <v>24</v>
       </c>
-      <c r="U25" s="92" t="n">
+      <c r="U25" s="93" t="n">
         <f aca="false">T25 - 2</f>
         <v>22</v>
       </c>
-      <c r="V25" s="92" t="n">
+      <c r="V25" s="93" t="n">
         <f aca="false">U25 - 2</f>
         <v>20</v>
       </c>
-      <c r="W25" s="20" t="n">
+      <c r="W25" s="21" t="n">
         <f aca="false">V25 - 2</f>
         <v>18</v>
       </c>
-      <c r="X25" s="93" t="n">
+      <c r="X25" s="94" t="n">
         <f aca="false">W25 - 2</f>
         <v>16</v>
       </c>
-      <c r="Y25" s="93" t="n">
+      <c r="Y25" s="94" t="n">
         <f aca="false">X25 - 2</f>
         <v>14</v>
       </c>
-      <c r="Z25" s="94" t="n">
+      <c r="Z25" s="95" t="n">
         <f aca="false">Y25 - 2</f>
         <v>12</v>
       </c>
-      <c r="AA25" s="94" t="n">
+      <c r="AA25" s="95" t="n">
         <f aca="false">Z25 - 2</f>
         <v>10</v>
       </c>
-      <c r="AB25" s="92" t="n">
+      <c r="AB25" s="93" t="n">
         <f aca="false">AA25 - 2</f>
         <v>8</v>
       </c>
-      <c r="AC25" s="92" t="n">
+      <c r="AC25" s="93" t="n">
         <f aca="false">AB25 - 2</f>
         <v>6</v>
       </c>
-      <c r="AD25" s="23" t="n">
+      <c r="AD25" s="24" t="n">
         <f aca="false">AC25 - 2</f>
         <v>4</v>
       </c>
-      <c r="AE25" s="24" t="n">
+      <c r="AE25" s="25" t="n">
         <f aca="false">AD25 - 2</f>
         <v>2</v>
       </c>
-      <c r="AF25" s="11"/>
-      <c r="AG25" s="11"/>
-      <c r="AI25" s="95"/>
+      <c r="AF25" s="12"/>
+      <c r="AG25" s="12"/>
+      <c r="AI25" s="96"/>
       <c r="AJ25" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI26" s="96"/>
+      <c r="AI26" s="97"/>
       <c r="AJ26" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI27" s="97"/>
+      <c r="AI27" s="98"/>
       <c r="AJ27" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F28" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI28" s="98"/>
+        <v>53</v>
+      </c>
+      <c r="AI28" s="99"/>
       <c r="AJ28" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI29" s="99"/>
+      <c r="AI29" s="100"/>
       <c r="AJ29" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI30" s="100"/>
+        <v>56</v>
+      </c>
+      <c r="AI30" s="101"/>
       <c r="AJ30" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI31" s="101"/>
+      <c r="AI31" s="102"/>
       <c r="AJ31" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI32" s="102"/>
+      <c r="AI32" s="103"/>
       <c r="AJ32" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
UPDATED DESIGN. LOST SPI0 to AD9361. DOES NOT GENERATE PROPER DEVICE TREE BLOB WITH AD9361 SUPPORT.
</commit_message>
<xml_diff>
--- a/ADRV9361z7035 BOB Pins.xlsx
+++ b/ADRV9361z7035 BOB Pins.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">RX</t>
   </si>
@@ -55,34 +55,28 @@
     <t xml:space="preserve">1.8 V</t>
   </si>
   <si>
-    <t xml:space="preserve">CS01</t>
+    <t xml:space="preserve">IO_L**_34_JX4_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO_L**_12_JX3_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO_L**_12_JX2_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC1</t>
   </si>
   <si>
     <t xml:space="preserve">SD1</t>
   </si>
   <si>
-    <t xml:space="preserve">IO_L**_34_JX4_*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO_L**_12_JX3_*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO_L**_12_JX2_*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MO0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI0</t>
+    <t xml:space="preserve">SC0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD0</t>
   </si>
   <si>
     <t xml:space="preserve">CLK0</t>
@@ -118,12 +112,6 @@
     <t xml:space="preserve">I2C SCL</t>
   </si>
   <si>
-    <t xml:space="preserve">SC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC0</t>
-  </si>
-  <si>
     <t xml:space="preserve">MI1</t>
   </si>
   <si>
@@ -155,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">IO_L**_MRCC_13_JX2_*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD0</t>
   </si>
   <si>
     <t xml:space="preserve">IO_L**_SRCC_13_JX2_*</t>
@@ -209,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -234,6 +219,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -511,7 +504,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -698,6 +691,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1008,7 +1005,7 @@
   <dimension ref="B2:AJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X29" activeCellId="0" sqref="X29"/>
+      <selection pane="topLeft" activeCell="AA9" activeCellId="0" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1337,8 +1334,8 @@
       <c r="J7" s="12" t="n">
         <v>967</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>11</v>
+      <c r="K7" s="12" t="n">
+        <v>991</v>
       </c>
       <c r="L7" s="12" t="n">
         <v>972</v>
@@ -1357,9 +1354,7 @@
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
-      <c r="U7" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="U7" s="12"/>
       <c r="V7" s="12" t="n">
         <v>979</v>
       </c>
@@ -1380,7 +1375,7 @@
       <c r="AG7" s="12"/>
       <c r="AI7" s="28"/>
       <c r="AJ7" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,7 +1450,7 @@
         <v>2</v>
       </c>
       <c r="Z8" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
@@ -1466,7 +1461,7 @@
       <c r="AG8" s="12"/>
       <c r="AI8" s="37"/>
       <c r="AJ8" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,10 +1546,10 @@
       <c r="AG9" s="12"/>
       <c r="AI9" s="46"/>
       <c r="AJ9" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -1565,25 +1560,25 @@
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
-      <c r="U10" s="12" t="s">
-        <v>21</v>
+      <c r="U10" s="47" t="s">
+        <v>19</v>
       </c>
       <c r="V10" s="12" t="n">
         <v>971</v>
@@ -1603,9 +1598,9 @@
       <c r="AE10" s="12"/>
       <c r="AF10" s="12"/>
       <c r="AG10" s="12"/>
-      <c r="AI10" s="47"/>
+      <c r="AI10" s="48"/>
       <c r="AJ10" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,19 +1633,19 @@
         <v>981</v>
       </c>
       <c r="R11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="V11" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="U11" s="0" t="s">
+      <c r="W11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="V11" s="0" t="s">
+      <c r="X11" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="W11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="X11" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
@@ -1659,9 +1654,9 @@
       <c r="AE11" s="12"/>
       <c r="AF11" s="12"/>
       <c r="AG11" s="12"/>
-      <c r="AI11" s="48"/>
+      <c r="AI11" s="49"/>
       <c r="AJ11" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,18 +1667,18 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="49" t="n">
+      <c r="I12" s="50" t="n">
         <v>32</v>
       </c>
-      <c r="J12" s="50" t="n">
+      <c r="J12" s="51" t="n">
         <f aca="false">I12 -2</f>
         <v>30</v>
       </c>
-      <c r="K12" s="51" t="n">
+      <c r="K12" s="52" t="n">
         <f aca="false">J12 -2</f>
         <v>28</v>
       </c>
-      <c r="L12" s="51" t="n">
+      <c r="L12" s="52" t="n">
         <f aca="false">K12 -2</f>
         <v>26</v>
       </c>
@@ -1691,7 +1686,7 @@
         <f aca="false">L12 -2</f>
         <v>24</v>
       </c>
-      <c r="N12" s="52" t="n">
+      <c r="N12" s="53" t="n">
         <f aca="false">M12 -2</f>
         <v>22</v>
       </c>
@@ -1731,13 +1726,13 @@
         <f aca="false">V12 -2</f>
         <v>4</v>
       </c>
-      <c r="X12" s="53" t="n">
+      <c r="X12" s="54" t="n">
         <f aca="false">W12 -2</f>
         <v>2</v>
       </c>
       <c r="Y12" s="12"/>
       <c r="Z12" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
@@ -1746,9 +1741,9 @@
       <c r="AE12" s="12"/>
       <c r="AF12" s="12"/>
       <c r="AG12" s="12"/>
-      <c r="AI12" s="54"/>
+      <c r="AI12" s="55"/>
       <c r="AJ12" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,10 +1754,10 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="55" t="n">
+      <c r="I13" s="56" t="n">
         <v>31</v>
       </c>
-      <c r="J13" s="56" t="n">
+      <c r="J13" s="57" t="n">
         <f aca="false">I13 - 2</f>
         <v>29</v>
       </c>
@@ -1774,15 +1769,15 @@
         <f aca="false">K13 - 2</f>
         <v>25</v>
       </c>
-      <c r="M13" s="57" t="n">
+      <c r="M13" s="58" t="n">
         <f aca="false">L13 - 2</f>
         <v>23</v>
       </c>
-      <c r="N13" s="57" t="n">
+      <c r="N13" s="58" t="n">
         <f aca="false">M13 - 2</f>
         <v>21</v>
       </c>
-      <c r="O13" s="58" t="n">
+      <c r="O13" s="59" t="n">
         <f aca="false">N13 - 2</f>
         <v>19</v>
       </c>
@@ -1798,7 +1793,7 @@
         <f aca="false">Q13 - 2</f>
         <v>13</v>
       </c>
-      <c r="S13" s="59" t="n">
+      <c r="S13" s="60" t="n">
         <f aca="false">R13 - 2</f>
         <v>11</v>
       </c>
@@ -1818,7 +1813,7 @@
         <f aca="false">V13 - 2</f>
         <v>3</v>
       </c>
-      <c r="X13" s="60" t="n">
+      <c r="X13" s="61" t="n">
         <f aca="false">W13 - 2</f>
         <v>1</v>
       </c>
@@ -1831,9 +1826,9 @@
       <c r="AE13" s="12"/>
       <c r="AF13" s="12"/>
       <c r="AG13" s="12"/>
-      <c r="AI13" s="61"/>
+      <c r="AI13" s="62"/>
       <c r="AJ13" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,15 +1839,9 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="J14" s="0" t="n">
         <v>980</v>
       </c>
-      <c r="K14" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="L14" s="0" t="n">
         <v>968</v>
       </c>
@@ -1887,7 +1876,7 @@
         <v>982</v>
       </c>
       <c r="X14" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
@@ -1896,9 +1885,9 @@
       <c r="AE14" s="12"/>
       <c r="AF14" s="12"/>
       <c r="AG14" s="12"/>
-      <c r="AI14" s="62"/>
+      <c r="AI14" s="63"/>
       <c r="AJ14" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,9 +1905,9 @@
       <c r="AE15" s="12"/>
       <c r="AF15" s="12"/>
       <c r="AG15" s="12"/>
-      <c r="AI15" s="63"/>
+      <c r="AI15" s="64"/>
       <c r="AJ15" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,72 +1918,72 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="64" t="n">
+      <c r="I16" s="65" t="n">
         <v>32</v>
       </c>
-      <c r="J16" s="65" t="n">
+      <c r="J16" s="66" t="n">
         <f aca="false">I16 -2</f>
         <v>30</v>
       </c>
-      <c r="K16" s="66" t="n">
+      <c r="K16" s="67" t="n">
         <f aca="false">J16 -2</f>
         <v>28</v>
       </c>
-      <c r="L16" s="66" t="n">
+      <c r="L16" s="67" t="n">
         <f aca="false">K16 -2</f>
         <v>26</v>
       </c>
-      <c r="M16" s="67" t="n">
+      <c r="M16" s="68" t="n">
         <f aca="false">L16 -2</f>
         <v>24</v>
       </c>
-      <c r="N16" s="67" t="n">
+      <c r="N16" s="68" t="n">
         <f aca="false">M16 -2</f>
         <v>22</v>
       </c>
-      <c r="O16" s="66" t="n">
+      <c r="O16" s="67" t="n">
         <f aca="false">N16 -2</f>
         <v>20</v>
       </c>
-      <c r="P16" s="66" t="n">
+      <c r="P16" s="67" t="n">
         <f aca="false">O16 -2</f>
         <v>18</v>
       </c>
-      <c r="Q16" s="66" t="n">
+      <c r="Q16" s="67" t="n">
         <f aca="false">P16 -2</f>
         <v>16</v>
       </c>
-      <c r="R16" s="66" t="n">
+      <c r="R16" s="67" t="n">
         <f aca="false">Q16 -2</f>
         <v>14</v>
       </c>
-      <c r="S16" s="68" t="n">
+      <c r="S16" s="69" t="n">
         <f aca="false">R16 -2</f>
         <v>12</v>
       </c>
-      <c r="T16" s="68" t="n">
+      <c r="T16" s="69" t="n">
         <f aca="false">S16 -2</f>
         <v>10</v>
       </c>
-      <c r="U16" s="66" t="n">
+      <c r="U16" s="67" t="n">
         <f aca="false">T16 -2</f>
         <v>8</v>
       </c>
-      <c r="V16" s="66" t="n">
+      <c r="V16" s="67" t="n">
         <f aca="false">U16 -2</f>
         <v>6</v>
       </c>
-      <c r="W16" s="66" t="n">
+      <c r="W16" s="67" t="n">
         <f aca="false">V16 -2</f>
         <v>4</v>
       </c>
-      <c r="X16" s="69" t="n">
+      <c r="X16" s="70" t="n">
         <f aca="false">W16 -2</f>
         <v>2</v>
       </c>
       <c r="Y16" s="12"/>
       <c r="Z16" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
@@ -2003,24 +1992,24 @@
       <c r="AE16" s="12"/>
       <c r="AF16" s="12"/>
       <c r="AG16" s="12"/>
-      <c r="AI16" s="70"/>
+      <c r="AI16" s="71"/>
       <c r="AJ16" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I17" s="71" t="n">
+      <c r="I17" s="72" t="n">
         <v>31</v>
       </c>
-      <c r="J17" s="72" t="n">
+      <c r="J17" s="73" t="n">
         <f aca="false">I17 - 2</f>
         <v>29</v>
       </c>
-      <c r="K17" s="73" t="n">
+      <c r="K17" s="74" t="n">
         <f aca="false">J17 - 2</f>
         <v>27</v>
       </c>
-      <c r="L17" s="73" t="n">
+      <c r="L17" s="74" t="n">
         <f aca="false">K17 - 2</f>
         <v>25</v>
       </c>
@@ -2032,19 +2021,19 @@
         <f aca="false">M17 - 2</f>
         <v>21</v>
       </c>
-      <c r="O17" s="73" t="n">
+      <c r="O17" s="74" t="n">
         <f aca="false">N17 - 2</f>
         <v>19</v>
       </c>
-      <c r="P17" s="73" t="n">
+      <c r="P17" s="74" t="n">
         <f aca="false">O17 - 2</f>
         <v>17</v>
       </c>
-      <c r="Q17" s="73" t="n">
+      <c r="Q17" s="74" t="n">
         <f aca="false">P17 - 2</f>
         <v>15</v>
       </c>
-      <c r="R17" s="73" t="n">
+      <c r="R17" s="74" t="n">
         <f aca="false">Q17 - 2</f>
         <v>13</v>
       </c>
@@ -2056,54 +2045,54 @@
         <f aca="false">S17 - 2</f>
         <v>9</v>
       </c>
-      <c r="U17" s="73" t="n">
+      <c r="U17" s="74" t="n">
         <f aca="false">T17 - 2</f>
         <v>7</v>
       </c>
-      <c r="V17" s="73" t="n">
+      <c r="V17" s="74" t="n">
         <f aca="false">U17 - 2</f>
         <v>5</v>
       </c>
-      <c r="W17" s="73" t="n">
+      <c r="W17" s="74" t="n">
         <f aca="false">V17 - 2</f>
         <v>3</v>
       </c>
-      <c r="X17" s="74" t="n">
+      <c r="X17" s="75" t="n">
         <f aca="false">W17 - 2</f>
         <v>1</v>
       </c>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
-      <c r="AI17" s="75"/>
+      <c r="AI17" s="76"/>
       <c r="AJ17" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI18" s="76"/>
+      <c r="AI18" s="77"/>
       <c r="AJ18" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI19" s="77"/>
+      <c r="AI19" s="78"/>
       <c r="AJ19" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="78" t="n">
+      <c r="I20" s="79" t="n">
         <v>32</v>
       </c>
-      <c r="J20" s="66" t="n">
+      <c r="J20" s="67" t="n">
         <f aca="false">I20 -2</f>
         <v>30</v>
       </c>
-      <c r="K20" s="66" t="n">
+      <c r="K20" s="67" t="n">
         <f aca="false">J20 -2</f>
         <v>28</v>
       </c>
-      <c r="L20" s="66" t="n">
+      <c r="L20" s="67" t="n">
         <f aca="false">K20 -2</f>
         <v>26</v>
       </c>
@@ -2111,23 +2100,23 @@
         <f aca="false">L20 -2</f>
         <v>24</v>
       </c>
-      <c r="N20" s="52" t="n">
+      <c r="N20" s="53" t="n">
         <f aca="false">M20 -2</f>
         <v>22</v>
       </c>
-      <c r="O20" s="66" t="n">
+      <c r="O20" s="67" t="n">
         <f aca="false">N20 -2</f>
         <v>20</v>
       </c>
-      <c r="P20" s="66" t="n">
+      <c r="P20" s="67" t="n">
         <f aca="false">O20 -2</f>
         <v>18</v>
       </c>
-      <c r="Q20" s="66" t="n">
+      <c r="Q20" s="67" t="n">
         <f aca="false">P20 -2</f>
         <v>16</v>
       </c>
-      <c r="R20" s="66" t="n">
+      <c r="R20" s="67" t="n">
         <f aca="false">Q20 -2</f>
         <v>14</v>
       </c>
@@ -2139,44 +2128,44 @@
         <f aca="false">S20 -2</f>
         <v>10</v>
       </c>
-      <c r="U20" s="66" t="n">
+      <c r="U20" s="67" t="n">
         <f aca="false">T20 -2</f>
         <v>8</v>
       </c>
-      <c r="V20" s="66" t="n">
+      <c r="V20" s="67" t="n">
         <f aca="false">U20 -2</f>
         <v>6</v>
       </c>
-      <c r="W20" s="66" t="n">
+      <c r="W20" s="67" t="n">
         <f aca="false">V20 -2</f>
         <v>4</v>
       </c>
-      <c r="X20" s="69" t="n">
+      <c r="X20" s="70" t="n">
         <f aca="false">W20 -2</f>
         <v>2</v>
       </c>
       <c r="Y20" s="12"/>
       <c r="Z20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI20" s="79"/>
+        <v>38</v>
+      </c>
+      <c r="AI20" s="80"/>
       <c r="AJ20" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="80" t="n">
+      <c r="I21" s="81" t="n">
         <v>31</v>
       </c>
-      <c r="J21" s="72" t="n">
+      <c r="J21" s="73" t="n">
         <f aca="false">I21 - 2</f>
         <v>29</v>
       </c>
-      <c r="K21" s="81" t="n">
+      <c r="K21" s="82" t="n">
         <f aca="false">J21 - 2</f>
         <v>27</v>
       </c>
-      <c r="L21" s="81" t="n">
+      <c r="L21" s="82" t="n">
         <f aca="false">K21 - 2</f>
         <v>25</v>
       </c>
@@ -2184,61 +2173,58 @@
         <f aca="false">L21 - 2</f>
         <v>23</v>
       </c>
-      <c r="N21" s="57" t="n">
+      <c r="N21" s="58" t="n">
         <f aca="false">M21 - 2</f>
         <v>21</v>
       </c>
-      <c r="O21" s="73" t="n">
+      <c r="O21" s="74" t="n">
         <f aca="false">N21 - 2</f>
         <v>19</v>
       </c>
-      <c r="P21" s="73" t="n">
+      <c r="P21" s="74" t="n">
         <f aca="false">O21 - 2</f>
         <v>17</v>
       </c>
-      <c r="Q21" s="73" t="n">
+      <c r="Q21" s="74" t="n">
         <f aca="false">P21 - 2</f>
         <v>15</v>
       </c>
-      <c r="R21" s="73" t="n">
+      <c r="R21" s="74" t="n">
         <f aca="false">Q21 - 2</f>
         <v>13</v>
       </c>
-      <c r="S21" s="57" t="n">
+      <c r="S21" s="58" t="n">
         <f aca="false">R21 - 2</f>
         <v>11</v>
       </c>
-      <c r="T21" s="57" t="n">
+      <c r="T21" s="58" t="n">
         <f aca="false">S21 - 2</f>
         <v>9</v>
       </c>
-      <c r="U21" s="73" t="n">
+      <c r="U21" s="74" t="n">
         <f aca="false">T21 - 2</f>
         <v>7</v>
       </c>
-      <c r="V21" s="73" t="n">
+      <c r="V21" s="74" t="n">
         <f aca="false">U21 - 2</f>
         <v>5</v>
       </c>
-      <c r="W21" s="73" t="n">
+      <c r="W21" s="74" t="n">
         <f aca="false">V21 - 2</f>
         <v>3</v>
       </c>
-      <c r="X21" s="74" t="n">
+      <c r="X21" s="75" t="n">
         <f aca="false">W21 - 2</f>
         <v>1</v>
       </c>
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
-      <c r="AI21" s="82"/>
+      <c r="AI21" s="83"/>
       <c r="AJ21" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M22" s="0" t="s">
-        <v>45</v>
-      </c>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N22" s="0" t="n">
         <v>906</v>
       </c>
@@ -2248,26 +2234,26 @@
       <c r="T22" s="0" t="n">
         <v>919</v>
       </c>
-      <c r="AI22" s="83"/>
+      <c r="AI22" s="84"/>
       <c r="AJ22" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI23" s="84"/>
+      <c r="AI23" s="85"/>
       <c r="AJ23" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="C24" s="85" t="n">
+      <c r="C24" s="86" t="n">
         <f aca="false">B24 - 2</f>
         <v>57</v>
       </c>
-      <c r="D24" s="85" t="n">
+      <c r="D24" s="86" t="n">
         <f aca="false">C24 - 2</f>
         <v>55</v>
       </c>
@@ -2275,27 +2261,27 @@
         <f aca="false">D24 - 2</f>
         <v>53</v>
       </c>
-      <c r="F24" s="86" t="n">
+      <c r="F24" s="87" t="n">
         <f aca="false">E24 - 2</f>
         <v>51</v>
       </c>
-      <c r="G24" s="86" t="n">
+      <c r="G24" s="87" t="n">
         <f aca="false">F24 - 2</f>
         <v>49</v>
       </c>
-      <c r="H24" s="86" t="n">
+      <c r="H24" s="87" t="n">
         <f aca="false">G24 - 2</f>
         <v>47</v>
       </c>
-      <c r="I24" s="86" t="n">
+      <c r="I24" s="87" t="n">
         <f aca="false">H24 - 2</f>
         <v>45</v>
       </c>
-      <c r="J24" s="86" t="n">
+      <c r="J24" s="87" t="n">
         <f aca="false">I24 - 2</f>
         <v>43</v>
       </c>
-      <c r="K24" s="86" t="n">
+      <c r="K24" s="87" t="n">
         <f aca="false">J24 - 2</f>
         <v>41</v>
       </c>
@@ -2303,43 +2289,43 @@
         <f aca="false">K24 - 2</f>
         <v>39</v>
       </c>
-      <c r="M24" s="87" t="n">
+      <c r="M24" s="88" t="n">
         <f aca="false">L24 - 2</f>
         <v>37</v>
       </c>
-      <c r="N24" s="87" t="n">
+      <c r="N24" s="88" t="n">
         <f aca="false">M24 - 2</f>
         <v>35</v>
       </c>
-      <c r="O24" s="87" t="n">
+      <c r="O24" s="88" t="n">
         <f aca="false">N24 - 2</f>
         <v>33</v>
       </c>
-      <c r="P24" s="87" t="n">
+      <c r="P24" s="88" t="n">
         <f aca="false">O24 - 2</f>
         <v>31</v>
       </c>
-      <c r="Q24" s="87" t="n">
+      <c r="Q24" s="88" t="n">
         <f aca="false">P24 - 2</f>
         <v>29</v>
       </c>
-      <c r="R24" s="87" t="n">
+      <c r="R24" s="88" t="n">
         <f aca="false">Q24 - 2</f>
         <v>27</v>
       </c>
-      <c r="S24" s="87" t="n">
+      <c r="S24" s="88" t="n">
         <f aca="false">R24 - 2</f>
         <v>25</v>
       </c>
-      <c r="T24" s="87" t="n">
+      <c r="T24" s="88" t="n">
         <f aca="false">S24 - 2</f>
         <v>23</v>
       </c>
-      <c r="U24" s="87" t="n">
+      <c r="U24" s="88" t="n">
         <f aca="false">T24 - 2</f>
         <v>21</v>
       </c>
-      <c r="V24" s="87" t="n">
+      <c r="V24" s="88" t="n">
         <f aca="false">U24 - 2</f>
         <v>19</v>
       </c>
@@ -2347,27 +2333,27 @@
         <f aca="false">V24 - 2</f>
         <v>17</v>
       </c>
-      <c r="X24" s="88" t="n">
+      <c r="X24" s="89" t="n">
         <f aca="false">W24 - 2</f>
         <v>15</v>
       </c>
-      <c r="Y24" s="88" t="n">
+      <c r="Y24" s="89" t="n">
         <f aca="false">X24 - 2</f>
         <v>13</v>
       </c>
-      <c r="Z24" s="89" t="n">
+      <c r="Z24" s="90" t="n">
         <f aca="false">Y24 - 2</f>
         <v>11</v>
       </c>
-      <c r="AA24" s="89" t="n">
+      <c r="AA24" s="90" t="n">
         <f aca="false">Z24 - 2</f>
         <v>9</v>
       </c>
-      <c r="AB24" s="87" t="n">
+      <c r="AB24" s="88" t="n">
         <f aca="false">AA24 - 2</f>
         <v>7</v>
       </c>
-      <c r="AC24" s="87" t="n">
+      <c r="AC24" s="88" t="n">
         <f aca="false">AB24 - 2</f>
         <v>5</v>
       </c>
@@ -2381,22 +2367,22 @@
       </c>
       <c r="AF24" s="12"/>
       <c r="AG24" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI24" s="90"/>
+        <v>43</v>
+      </c>
+      <c r="AI24" s="91"/>
       <c r="AJ24" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="15" t="n">
         <v>60</v>
       </c>
-      <c r="C25" s="91" t="n">
+      <c r="C25" s="92" t="n">
         <f aca="false">B25 - 2</f>
         <v>58</v>
       </c>
-      <c r="D25" s="91" t="n">
+      <c r="D25" s="92" t="n">
         <f aca="false">C25 - 2</f>
         <v>56</v>
       </c>
@@ -2404,27 +2390,27 @@
         <f aca="false">D25 - 2</f>
         <v>54</v>
       </c>
-      <c r="F25" s="92" t="n">
+      <c r="F25" s="93" t="n">
         <f aca="false">E25 - 2</f>
         <v>52</v>
       </c>
-      <c r="G25" s="92" t="n">
+      <c r="G25" s="93" t="n">
         <f aca="false">F25 - 2</f>
         <v>50</v>
       </c>
-      <c r="H25" s="92" t="n">
+      <c r="H25" s="93" t="n">
         <f aca="false">G25 - 2</f>
         <v>48</v>
       </c>
-      <c r="I25" s="92" t="n">
+      <c r="I25" s="93" t="n">
         <f aca="false">H25 - 2</f>
         <v>46</v>
       </c>
-      <c r="J25" s="92" t="n">
+      <c r="J25" s="93" t="n">
         <f aca="false">I25 - 2</f>
         <v>44</v>
       </c>
-      <c r="K25" s="92" t="n">
+      <c r="K25" s="93" t="n">
         <f aca="false">J25 - 2</f>
         <v>42</v>
       </c>
@@ -2432,43 +2418,43 @@
         <f aca="false">K25 - 2</f>
         <v>40</v>
       </c>
-      <c r="M25" s="93" t="n">
+      <c r="M25" s="94" t="n">
         <f aca="false">L25 - 2</f>
         <v>38</v>
       </c>
-      <c r="N25" s="93" t="n">
+      <c r="N25" s="94" t="n">
         <f aca="false">M25 - 2</f>
         <v>36</v>
       </c>
-      <c r="O25" s="93" t="n">
+      <c r="O25" s="94" t="n">
         <f aca="false">N25 - 2</f>
         <v>34</v>
       </c>
-      <c r="P25" s="93" t="n">
+      <c r="P25" s="94" t="n">
         <f aca="false">O25 - 2</f>
         <v>32</v>
       </c>
-      <c r="Q25" s="93" t="n">
+      <c r="Q25" s="94" t="n">
         <f aca="false">P25 - 2</f>
         <v>30</v>
       </c>
-      <c r="R25" s="93" t="n">
+      <c r="R25" s="94" t="n">
         <f aca="false">Q25 - 2</f>
         <v>28</v>
       </c>
-      <c r="S25" s="93" t="n">
+      <c r="S25" s="94" t="n">
         <f aca="false">R25 - 2</f>
         <v>26</v>
       </c>
-      <c r="T25" s="93" t="n">
+      <c r="T25" s="94" t="n">
         <f aca="false">S25 - 2</f>
         <v>24</v>
       </c>
-      <c r="U25" s="93" t="n">
+      <c r="U25" s="94" t="n">
         <f aca="false">T25 - 2</f>
         <v>22</v>
       </c>
-      <c r="V25" s="93" t="n">
+      <c r="V25" s="94" t="n">
         <f aca="false">U25 - 2</f>
         <v>20</v>
       </c>
@@ -2476,27 +2462,27 @@
         <f aca="false">V25 - 2</f>
         <v>18</v>
       </c>
-      <c r="X25" s="94" t="n">
+      <c r="X25" s="95" t="n">
         <f aca="false">W25 - 2</f>
         <v>16</v>
       </c>
-      <c r="Y25" s="94" t="n">
+      <c r="Y25" s="95" t="n">
         <f aca="false">X25 - 2</f>
         <v>14</v>
       </c>
-      <c r="Z25" s="95" t="n">
+      <c r="Z25" s="96" t="n">
         <f aca="false">Y25 - 2</f>
         <v>12</v>
       </c>
-      <c r="AA25" s="95" t="n">
+      <c r="AA25" s="96" t="n">
         <f aca="false">Z25 - 2</f>
         <v>10</v>
       </c>
-      <c r="AB25" s="93" t="n">
+      <c r="AB25" s="94" t="n">
         <f aca="false">AA25 - 2</f>
         <v>8</v>
       </c>
-      <c r="AC25" s="93" t="n">
+      <c r="AC25" s="94" t="n">
         <f aca="false">AB25 - 2</f>
         <v>6</v>
       </c>
@@ -2510,57 +2496,57 @@
       </c>
       <c r="AF25" s="12"/>
       <c r="AG25" s="12"/>
-      <c r="AI25" s="96"/>
+      <c r="AI25" s="97"/>
       <c r="AJ25" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI26" s="97"/>
+      <c r="AI26" s="98"/>
       <c r="AJ26" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI27" s="98"/>
+      <c r="AI27" s="99"/>
       <c r="AJ27" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F28" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI28" s="99"/>
+        <v>48</v>
+      </c>
+      <c r="AI28" s="100"/>
       <c r="AJ28" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI29" s="100"/>
+      <c r="AI29" s="101"/>
       <c r="AJ29" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI30" s="101"/>
+        <v>51</v>
+      </c>
+      <c r="AI30" s="102"/>
       <c r="AJ30" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI31" s="102"/>
+      <c r="AI31" s="103"/>
       <c r="AJ31" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AI32" s="103"/>
+      <c r="AI32" s="104"/>
       <c r="AJ32" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>